<commit_message>
Memperbaiki rombel di SiswaController; mengubah cetak raport untuk menampilkan rombel; edit di isian perubahan data nilai
</commit_message>
<xml_diff>
--- a/public/file_nilai/nilai_kelas2_form.xlsx
+++ b/public/file_nilai/nilai_kelas2_form.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\pbpm\public\file_nilai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476EC70-141D-4E5E-AA00-54F3F8477D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F63EB8-010B-4642-89C1-59C0393F4123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27260" yWindow="-114" windowWidth="27603" windowHeight="14927" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2990,13 +2990,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>

</xml_diff>